<commit_message>
Undef var err code
</commit_message>
<xml_diff>
--- a/LL_GRAMMAR.xlsx
+++ b/LL_GRAMMAR.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{204501B0-A2C9-4039-A513-83B50AF3412C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\C\IFJ_PROJECT\ifj-project-2022\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842C8E83-BFBA-47F8-BC1F-A0E0FDFC9145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -28,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>&lt;PROG&gt;</t>
   </si>
   <si>
-    <t>&lt;DECLARE&gt; ; &lt;ST_L&gt; &lt;OPT_EOF&gt;</t>
-  </si>
-  <si>
     <t>&lt;DECLARE&gt;</t>
   </si>
   <si>
@@ -60,9 +62,6 @@
     <t>if ( &lt;STAT_INSIDE&gt; ) { &lt;ST_L&gt; } &lt;ELSE&gt;</t>
   </si>
   <si>
-    <t>while ( \EXPRESSION_PARSER ) { &lt;ST_L&gt; }</t>
-  </si>
-  <si>
     <t>function ID ( &lt;PARAMS&gt; ) : &lt;RET_TYPE&gt; { &lt;ST_L&gt; }</t>
   </si>
   <si>
@@ -84,9 +83,6 @@
     <t>&lt;STAT_INSIDE&gt;</t>
   </si>
   <si>
-    <t>\EXPRESSION_PARSER</t>
-  </si>
-  <si>
     <t>&lt;PARAMS&gt;</t>
   </si>
   <si>
@@ -124,13 +120,25 @@
   </si>
   <si>
     <t>void</t>
+  </si>
+  <si>
+    <t>\EXPRESSION_PARSER\</t>
+  </si>
+  <si>
+    <t>while ( \EXPRESSION_PARSER\ ) { &lt;ST_L&gt; }</t>
+  </si>
+  <si>
+    <t>&lt;?php &lt;DECLARE&gt; ; &lt;ST_L&gt; &lt;OPT_EOF&gt;</t>
+  </si>
+  <si>
+    <t>? &lt;TYPE&gt; &lt;SEP&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,14 +147,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Daytona"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Daytona"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Daytona"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,12 +175,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDBDBDB"/>
+        <fgColor rgb="FFF2F8EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5E8CA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -342,55 +368,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -399,6 +440,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD5E8CA"/>
+      <color rgb="FFF2F8EE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -411,7 +458,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -699,7 +746,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -707,345 +754,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="B2:I25"/>
+      <selection activeCell="J1" sqref="J1:J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="20.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="20.25" customHeight="1">
+    <row r="1" spans="1:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B10" s="5" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B13" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B14" s="5" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B18" s="5" t="s">
+      <c r="C21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B19" s="5" t="s">
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B20" s="5" t="s">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B21" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="1:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B22" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:10" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B25" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
@@ -1053,9 +1160,38 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="15"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="28">
+    <mergeCell ref="J1:J26"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A1:A25"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C3:I3"/>
@@ -1068,19 +1204,8 @@
     <mergeCell ref="C10:I10"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="C12:I12"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>